<commit_message>
Enums bearbeitet und UnitTests erstellt
</commit_message>
<xml_diff>
--- a/src/specification/MTCG_Checklist_final.xlsx
+++ b/src/specification/MTCG_Checklist_final.xlsx
@@ -1,31 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wallisch\Nextcloud\Lehre\S3-SWEN1\Semester-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bsnyr/Documents/01FHLocal/03Semester/SWEN/MonsterTradingCardsGame/src/specification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C8C713-8F7F-4CDE-8F5E-C0683C55AF63}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{033C9276-2AFA-C149-A000-E941CDC21716}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9580" windowHeight="8040" xr2:uid="{88369686-F968-45CB-887F-E38F2E727DD7}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="21080" xr2:uid="{88369686-F968-45CB-887F-E38F2E727DD7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="54">
   <si>
     <t>Checklist MonsterTradingCardsGame</t>
   </si>
@@ -123,9 +134,6 @@
     <t>Non-functional Requirements</t>
   </si>
   <si>
-    <t>Token-based security</t>
-  </si>
-  <si>
     <t>Persistence (DB)</t>
   </si>
   <si>
@@ -184,6 +192,12 @@
   </si>
   <si>
     <t>All REST API Endpoints defined accoring to specs</t>
+  </si>
+  <si>
+    <t>‚‚‚</t>
+  </si>
+  <si>
+    <t>done</t>
   </si>
 </sst>
 </file>
@@ -291,7 +305,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -325,9 +339,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -365,7 +379,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -471,7 +485,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -613,7 +627,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -623,43 +637,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D58600B0-3567-4A3D-A785-925E0537D06D}">
   <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="137" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="68" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:4" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="1" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
@@ -667,63 +681,84 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>12</v>
       </c>
@@ -731,12 +766,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="4" customFormat="1" ht="21" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:4" s="4" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:4" s="1" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
         <v>14</v>
       </c>
@@ -747,61 +782,76 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:4" s="1" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B20"/>
       <c r="C20"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B21" s="9"/>
       <c r="C21" s="6"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D21" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B22" s="9"/>
       <c r="C22" s="6"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D22" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B23" s="9"/>
       <c r="C23" s="6"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D23" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B24" s="9"/>
       <c r="C24" s="6"/>
-    </row>
-    <row r="26" spans="1:4" s="1" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D24" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B27" s="9"/>
       <c r="C27" s="6"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B28" s="9"/>
       <c r="C28" s="6"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D28" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
         <v>18</v>
       </c>
@@ -809,7 +859,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
         <v>19</v>
       </c>
@@ -817,7 +867,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
         <v>20</v>
       </c>
@@ -825,7 +875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
         <v>21</v>
       </c>
@@ -833,7 +883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
         <v>22</v>
       </c>
@@ -841,14 +891,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:3" s="1" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B35"/>
       <c r="C35"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
         <v>24</v>
       </c>
@@ -856,7 +906,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
         <v>25</v>
       </c>
@@ -864,7 +914,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
         <v>26</v>
       </c>
@@ -872,7 +922,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
         <v>27</v>
       </c>
@@ -880,7 +930,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
         <v>28</v>
       </c>
@@ -888,7 +938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
         <v>29</v>
       </c>
@@ -896,7 +946,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:3" s="1" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>30</v>
       </c>
@@ -905,108 +955,108 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:3" s="1" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B45"/>
       <c r="C45"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="B46" s="9"/>
       <c r="C46" s="6"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C47" s="6">
         <v>8</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C48" s="6">
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C49" s="6">
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:3" s="1" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B51"/>
       <c r="C51" s="6"/>
     </row>
-    <row r="53" spans="1:3" s="1" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B53" s="7"/>
       <c r="C53" s="7"/>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C54" s="6">
         <v>0.5</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C55" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C56" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C57" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C58" s="6">
         <v>0.5</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B59" s="9"/>
       <c r="C59" s="6"/>
     </row>
-    <row r="61" spans="1:3" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.5">
+    <row r="61" spans="1:3" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B61" s="2">
         <f>IF(MIN(B9:B16)=1,SUM(B28:B59),0)</f>
@@ -1029,6 +1079,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100495F7CC252815B47896F98900E10984C" ma:contentTypeVersion="2" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="afe1b3b164495dc81fdbcdcad6ec8b68">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="207955a2-a3fc-4582-b2ea-e4c7d1fb6048" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3b6a42bf87c3f8727d31c248fc1697f6" ns2:_="">
     <xsd:import namespace="207955a2-a3fc-4582-b2ea-e4c7d1fb6048"/>
@@ -1160,22 +1225,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5FFD0135-03B1-4A6A-9DC8-B4D791C0671E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="207955a2-a3fc-4582-b2ea-e4c7d1fb6048"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B871BF9-5772-4B74-B6DF-7878EF29873D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0824ED0-660A-437B-A039-7835C5DD208D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1191,28 +1265,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B871BF9-5772-4B74-B6DF-7878EF29873D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5FFD0135-03B1-4A6A-9DC8-B4D791C0671E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="207955a2-a3fc-4582-b2ea-e4c7d1fb6048"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
current state with the problems in Deck
</commit_message>
<xml_diff>
--- a/src/specification/MTCG_Checklist_final.xlsx
+++ b/src/specification/MTCG_Checklist_final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bsnyr/Documents/01FHLocal/03Semester/SWEN/MonsterTradingCardsGame/src/specification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{033C9276-2AFA-C149-A000-E941CDC21716}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5C6D959-FDB8-6B47-A1FC-E71F28021008}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="21080" xr2:uid="{88369686-F968-45CB-887F-E38F2E727DD7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="54">
   <si>
     <t>Checklist MonsterTradingCardsGame</t>
   </si>
@@ -637,8 +637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D58600B0-3567-4A3D-A785-925E0537D06D}">
   <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="137" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="137" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -857,6 +857,9 @@
       </c>
       <c r="C29" s="6">
         <v>2</v>
+      </c>
+      <c r="D29" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
current state with started BattleLogic
</commit_message>
<xml_diff>
--- a/src/specification/MTCG_Checklist_final.xlsx
+++ b/src/specification/MTCG_Checklist_final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bsnyr/Documents/01FHLocal/03Semester/SWEN/MonsterTradingCardsGame/src/specification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5C6D959-FDB8-6B47-A1FC-E71F28021008}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74EBC73F-58C6-E740-A0F6-56D0A7089277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="21080" xr2:uid="{88369686-F968-45CB-887F-E38F2E727DD7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="54">
   <si>
     <t>Checklist MonsterTradingCardsGame</t>
   </si>
@@ -637,8 +637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D58600B0-3567-4A3D-A785-925E0537D06D}">
   <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="137" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="137" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -869,6 +869,9 @@
       <c r="C30" s="6">
         <v>2</v>
       </c>
+      <c r="D30" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
@@ -886,7 +889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
         <v>22</v>
       </c>
@@ -894,14 +897,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:3" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B35"/>
       <c r="C35"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
         <v>24</v>
       </c>
@@ -909,7 +912,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
         <v>25</v>
       </c>
@@ -917,7 +920,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
         <v>26</v>
       </c>
@@ -925,7 +928,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
         <v>27</v>
       </c>
@@ -933,7 +936,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
         <v>28</v>
       </c>
@@ -941,7 +944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
         <v>29</v>
       </c>
@@ -949,7 +952,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:3" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>30</v>
       </c>
@@ -958,29 +961,32 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:3" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B45"/>
       <c r="C45"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
         <v>52</v>
       </c>
       <c r="B46" s="9"/>
       <c r="C46" s="6"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="s">
         <v>32</v>
       </c>
       <c r="C47" s="6">
         <v>8</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D47" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="s">
         <v>44</v>
       </c>

</xml_diff>

<commit_message>
current state with problems
</commit_message>
<xml_diff>
--- a/src/specification/MTCG_Checklist_final.xlsx
+++ b/src/specification/MTCG_Checklist_final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bsnyr/Documents/01FHLocal/03Semester/SWEN/MonsterTradingCardsGame/src/specification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFAD0336-C2BC-FE47-ACBF-16F298FCE1EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B74EDFBC-DCC8-7244-9A7A-24589B98E2FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="21080" xr2:uid="{88369686-F968-45CB-887F-E38F2E727DD7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="55">
   <si>
     <t>Checklist MonsterTradingCardsGame</t>
   </si>
@@ -198,6 +198,9 @@
   </si>
   <si>
     <t>done</t>
+  </si>
+  <si>
+    <t>will not be made</t>
   </si>
 </sst>
 </file>
@@ -637,8 +640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D58600B0-3567-4A3D-A785-925E0537D06D}">
   <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="137" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="137" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -901,6 +904,9 @@
       </c>
       <c r="C33" s="6">
         <v>3</v>
+      </c>
+      <c r="D33" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="35" spans="1:4" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">

</xml_diff>